<commit_message>
0.7.5 - optimisation and parametric simulation
</commit_message>
<xml_diff>
--- a/WIP_outputs.xlsx
+++ b/WIP_outputs.xlsx
@@ -97,16 +97,16 @@
     <t>[11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.490694444444445, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.592361111111112, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.412962962962967, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.138472222222221, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 11.000601851851853, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.888912037037036, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.809699074074077, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.716898148148147, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.537060185185185, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.30173611111111, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.164097222222223, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 10.009004629629631, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.859537037037041, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.825069444444447, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.605000000000002, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.431018518518519, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.32886574074074, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.41965277777778, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.469791666666671, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.368125000000004, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.306875000000003, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.189976851851851, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.132037037037039, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.091388888888893, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.205231481481484, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.42476851851852, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.592800925925928, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.657685185185189, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.733657407407408, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 9.944398148148151, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.238449074074078, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.208425925925928, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.223634259259262, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.299375000000003, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.383865740740744, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.418703703703706, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.446898148148149, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.52803240740741, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.62638888888889, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.792222222222222, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 10.916527777777775, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.119166666666665, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.265578703703701, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.360023148148144, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.525578703703701, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.658263888888884, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.791388888888887, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.672407407407405, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.548888888888884, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.648657407407404, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.681805555555554, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.787129629629627, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 11.87784722222222, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 12.01594907407407, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.891273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.696273148148146, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.634259259259258, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.645439814814814, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.809791666666664, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.906064814814814, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.656203703703705, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.396828703703706, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.445092592592596, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.579490740740743, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.644351851851853, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.719861111111113, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.779861111111112, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.822685185185184, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.916990740740742, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.993379629629631, 11.9933796</t>
   </si>
   <si>
-    <t>WIP_testing predefined models\BESOS_Output\6GAA8Y9JI3LRNPEI9TAZ</t>
-  </si>
-  <si>
-    <t>WIP_testing predefined models\BESOS_Output\J9B4JGZ6CFXIB3AXNS3A</t>
-  </si>
-  <si>
-    <t>WIP_testing predefined models\BESOS_Output\TBGDB71MYES71LDH06YG</t>
-  </si>
-  <si>
-    <t>WIP_testing predefined models\BESOS_Output\1LY192ARJY3LH66IRQ3B</t>
+    <t>WIP_testing predefined models\BESOS_Output\X4E19VWN0PTA2159A5GZ</t>
+  </si>
+  <si>
+    <t>WIP_testing predefined models\BESOS_Output\A6SWO6FY6Z7J0MVGCRJK</t>
+  </si>
+  <si>
+    <t>WIP_testing predefined models\BESOS_Output\YQJC31UPERDY6A8NBE84</t>
+  </si>
+  <si>
+    <t>WIP_testing predefined models\BESOS_Output\SJ47E8CQWB3RUHK3GJ6I</t>
   </si>
   <si>
     <t>Sydney</t>

</xml_diff>